<commit_message>
Partially working show all
</commit_message>
<xml_diff>
--- a/00_Raw_Assets/quotes_v1.xlsx
+++ b/00_Raw_Assets/quotes_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\01_GK_Tutorials\12_91902_Quotes_DB\00_Raw_Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\01_GK_Tutorials\13_91902_Quotes_DB\00_Raw_Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E6AD78-F27F-413A-BA0C-6151542442AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001769BF-4FC2-4F72-BE25-B30B01970BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -1958,9 +1958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5900,7 +5900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>

</xml_diff>